<commit_message>
updated bucket list; Note: at this state, system was tested with 200 process's and it worked!
</commit_message>
<xml_diff>
--- a/check list.xlsx
+++ b/check list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ml170\OneDrive\Desktop\os1 projekat pokusaji\so1 git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FC2A84-EE1E-405D-95EF-2660DAF59007}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115C559C-4C75-402A-BAD4-C5321A517CFA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="2400" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="20">
   <si>
     <t>implementation</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>─</t>
-  </si>
-  <si>
-    <t>no</t>
   </si>
 </sst>
 </file>
@@ -129,9 +126,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,7 +414,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,6 +422,7 @@
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="12.88671875" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -452,8 +452,8 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
+      <c r="E2" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -469,8 +469,8 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
+      <c r="E3" s="3">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -487,7 +487,7 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>